<commit_message>
commit version2  with changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TechBloomersDsalgo.xlsx
+++ b/src/test/resources/testdata/TechBloomersDsalgo.xlsx
@@ -4,18 +4,23 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="10960"/>
+    <workbookView windowWidth="28800" windowHeight="10960" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="ArraypythonCode" sheetId="1" r:id="rId2"/>
+    <sheet name="TreepythonCode" sheetId="3" r:id="rId3"/>
+    <sheet name="GraphpythonCode" sheetId="4" r:id="rId4"/>
+    <sheet name="StackpythonCode" sheetId="5" r:id="rId5"/>
+    <sheet name="Queuecode" sheetId="6" r:id="rId6"/>
+    <sheet name="Linkedlistcode" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
   <si>
     <t>username</t>
   </si>
@@ -145,6 +150,36 @@
   </si>
   <si>
     <t>submission success</t>
+  </si>
+  <si>
+    <t>TreepythonCode</t>
+  </si>
+  <si>
+    <t>print("This is Tree in python")</t>
+  </si>
+  <si>
+    <t>GraphpythonCode</t>
+  </si>
+  <si>
+    <t>print("This is Graph in python")</t>
+  </si>
+  <si>
+    <t>StackpythonCode</t>
+  </si>
+  <si>
+    <t>print("This is Stack in python")</t>
+  </si>
+  <si>
+    <t>Queuecode</t>
+  </si>
+  <si>
+    <t>print("This is Queue in python")</t>
+  </si>
+  <si>
+    <t>Linkedlistcode</t>
+  </si>
+  <si>
+    <t>print("This is LinkedList in python")</t>
   </si>
 </sst>
 </file>
@@ -771,10 +806,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1107,8 +1142,8 @@
   <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="2"/>
@@ -1209,8 +1244,8 @@
   <sheetPr/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="1"/>
@@ -1220,18 +1255,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" ht="28" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1239,18 +1274,18 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" ht="224" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" ht="266" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B5">
@@ -1258,7 +1293,7 @@
       </c>
     </row>
     <row r="6" ht="196" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B6">
@@ -1266,7 +1301,7 @@
       </c>
     </row>
     <row r="7" ht="154" spans="1:2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B7" t="s">
@@ -1274,11 +1309,189 @@
       </c>
     </row>
     <row r="8" ht="168" spans="1:2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" ht="28" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3">
+      <c r="C6" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" ht="28" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" ht="28" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" ht="28" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" ht="42" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>